<commit_message>
last trimming & fastqc update.
</commit_message>
<xml_diff>
--- a/Bioinformatics/2-Trimming/fastp/Trimming_Info.xlsx
+++ b/Bioinformatics/2-Trimming/fastp/Trimming_Info.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="rnasep1" sheetId="2" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="73">
   <si>
     <t>Sample</t>
   </si>
@@ -231,6 +231,9 @@
   </si>
   <si>
     <t>AVRX-28b</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -266,8 +269,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -574,8 +580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -621,21 +627,21 @@
         <v>9740360</v>
       </c>
       <c r="D2">
-        <v>4411102</v>
+        <v>4661816</v>
       </c>
       <c r="E2">
-        <v>4411102</v>
+        <v>4661816</v>
       </c>
       <c r="F2">
-        <v>584832</v>
+        <v>312986</v>
       </c>
       <c r="G2">
         <f>(D2*100)/B2</f>
-        <v>45.286847714047532</v>
+        <v>47.860818285977111</v>
       </c>
       <c r="H2">
         <f>100-G2</f>
-        <v>54.713152285952468</v>
+        <v>52.139181714022889</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -649,21 +655,21 @@
         <v>10263013</v>
       </c>
       <c r="D3">
-        <v>4797547</v>
+        <v>5057036</v>
       </c>
       <c r="E3">
-        <v>4797547</v>
+        <v>5057036</v>
       </c>
       <c r="F3">
-        <v>381214</v>
+        <v>222388</v>
       </c>
       <c r="G3">
         <f t="shared" ref="G3:G37" si="0">(D3*100)/B3</f>
-        <v>46.745989701075111</v>
+        <v>49.2743797557306</v>
       </c>
       <c r="H3">
         <f t="shared" ref="H3:H37" si="1">100-G3</f>
-        <v>53.254010298924889</v>
+        <v>50.7256202442694</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
@@ -677,21 +683,21 @@
         <v>10611540</v>
       </c>
       <c r="D4">
-        <v>4821548</v>
+        <v>5091448</v>
       </c>
       <c r="E4">
-        <v>4821548</v>
+        <v>5091448</v>
       </c>
       <c r="F4">
-        <v>697446</v>
+        <v>369806</v>
       </c>
       <c r="G4">
         <f t="shared" si="0"/>
-        <v>45.43683574674364</v>
+        <v>47.980293152549017</v>
       </c>
       <c r="H4">
         <f t="shared" si="1"/>
-        <v>54.56316425325636</v>
+        <v>52.019706847450983</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
@@ -705,21 +711,21 @@
         <v>12128425</v>
       </c>
       <c r="D5">
-        <v>5791549</v>
+        <v>6105833</v>
       </c>
       <c r="E5">
-        <v>5791549</v>
+        <v>6105833</v>
       </c>
       <c r="F5">
-        <v>588326</v>
+        <v>365390</v>
       </c>
       <c r="G5">
         <f t="shared" si="0"/>
-        <v>47.751863906484147</v>
+        <v>50.343164920424542</v>
       </c>
       <c r="H5">
         <f t="shared" si="1"/>
-        <v>52.248136093515853</v>
+        <v>49.656835079575458</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
@@ -733,21 +739,21 @@
         <v>11178989</v>
       </c>
       <c r="D6">
-        <v>5365019</v>
+        <v>5627016</v>
       </c>
       <c r="E6">
-        <v>5365019</v>
+        <v>5627016</v>
       </c>
       <c r="F6">
-        <v>386800</v>
+        <v>270958</v>
       </c>
       <c r="G6">
         <f t="shared" si="0"/>
-        <v>47.991987468634235</v>
+        <v>50.335643053231379</v>
       </c>
       <c r="H6">
         <f t="shared" si="1"/>
-        <v>52.008012531365765</v>
+        <v>49.664356946768621</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
@@ -761,21 +767,21 @@
         <v>9905809</v>
       </c>
       <c r="D7">
-        <v>4300641</v>
+        <v>4551280</v>
       </c>
       <c r="E7">
-        <v>4300641</v>
+        <v>4551280</v>
       </c>
       <c r="F7">
-        <v>283854</v>
+        <v>173440</v>
       </c>
       <c r="G7">
         <f t="shared" si="0"/>
-        <v>43.41534346159915</v>
+        <v>45.945565879576314</v>
       </c>
       <c r="H7">
         <f t="shared" si="1"/>
-        <v>56.58465653840085</v>
+        <v>54.054434120423686</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
@@ -789,21 +795,21 @@
         <v>10468691</v>
       </c>
       <c r="D8">
-        <v>4858082</v>
+        <v>5126912</v>
       </c>
       <c r="E8">
-        <v>4858082</v>
+        <v>5126912</v>
       </c>
       <c r="F8">
-        <v>463716</v>
+        <v>277676</v>
       </c>
       <c r="G8">
         <f t="shared" si="0"/>
-        <v>46.405820937880392</v>
+        <v>48.973763768555209</v>
       </c>
       <c r="H8">
         <f t="shared" si="1"/>
-        <v>53.594179062119608</v>
+        <v>51.026236231444791</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
@@ -817,21 +823,21 @@
         <v>9860841</v>
       </c>
       <c r="D9">
-        <v>4444037</v>
+        <v>4694382</v>
       </c>
       <c r="E9">
-        <v>4444037</v>
+        <v>4694382</v>
       </c>
       <c r="F9">
-        <v>246212</v>
+        <v>153910</v>
       </c>
       <c r="G9">
         <f t="shared" si="0"/>
-        <v>45.067525173562785</v>
+        <v>47.606304573818804</v>
       </c>
       <c r="H9">
         <f t="shared" si="1"/>
-        <v>54.932474826437215</v>
+        <v>52.393695426181196</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
@@ -845,21 +851,21 @@
         <v>9705114</v>
       </c>
       <c r="D10">
-        <v>4354919</v>
+        <v>4603532</v>
       </c>
       <c r="E10">
-        <v>4354919</v>
+        <v>4603532</v>
       </c>
       <c r="F10">
-        <v>387858</v>
+        <v>215642</v>
       </c>
       <c r="G10">
         <f t="shared" si="0"/>
-        <v>44.872414687761527</v>
+        <v>47.434084751606214</v>
       </c>
       <c r="H10">
         <f t="shared" si="1"/>
-        <v>55.127585312238473</v>
+        <v>52.565915248393786</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
@@ -873,21 +879,21 @@
         <v>10850413</v>
       </c>
       <c r="D11">
-        <v>4438437</v>
+        <v>4684565</v>
       </c>
       <c r="E11">
-        <v>4438437</v>
+        <v>4684565</v>
       </c>
       <c r="F11">
-        <v>235148</v>
+        <v>141736</v>
       </c>
       <c r="G11">
         <f t="shared" si="0"/>
-        <v>40.905696400680782</v>
+        <v>43.174070885596706</v>
       </c>
       <c r="H11">
         <f t="shared" si="1"/>
-        <v>59.094303599319218</v>
+        <v>56.825929114403294</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
@@ -901,21 +907,21 @@
         <v>10641598</v>
       </c>
       <c r="D12">
-        <v>5142842</v>
+        <v>5412989</v>
       </c>
       <c r="E12">
-        <v>5142842</v>
+        <v>5412989</v>
       </c>
       <c r="F12">
-        <v>756896</v>
+        <v>417306</v>
       </c>
       <c r="G12">
         <f t="shared" si="0"/>
-        <v>48.327722960405005</v>
+        <v>50.866317257990765</v>
       </c>
       <c r="H12">
         <f t="shared" si="1"/>
-        <v>51.672277039594995</v>
+        <v>49.133682742009235</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
@@ -929,21 +935,21 @@
         <v>8817983</v>
       </c>
       <c r="D13">
-        <v>4174874</v>
+        <v>4406925</v>
       </c>
       <c r="E13">
-        <v>4174874</v>
+        <v>4406925</v>
       </c>
       <c r="F13">
-        <v>251820</v>
+        <v>149966</v>
       </c>
       <c r="G13">
         <f t="shared" si="0"/>
-        <v>47.344999417667282</v>
+        <v>49.976564935541383</v>
       </c>
       <c r="H13">
         <f t="shared" si="1"/>
-        <v>52.655000582332718</v>
+        <v>50.023435064458617</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
@@ -957,21 +963,21 @@
         <v>12097979</v>
       </c>
       <c r="D14">
-        <v>5384628</v>
+        <v>5677991</v>
       </c>
       <c r="E14">
-        <v>5384628</v>
+        <v>5677991</v>
       </c>
       <c r="F14">
-        <v>524876</v>
+        <v>296754</v>
       </c>
       <c r="G14">
         <f t="shared" si="0"/>
-        <v>44.508491872898773</v>
+        <v>46.933384493393483</v>
       </c>
       <c r="H14">
         <f t="shared" si="1"/>
-        <v>55.491508127101227</v>
+        <v>53.066615506606517</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
@@ -985,21 +991,21 @@
         <v>10288037</v>
       </c>
       <c r="D15">
-        <v>4880188</v>
+        <v>5131527</v>
       </c>
       <c r="E15">
-        <v>4880188</v>
+        <v>5131527</v>
       </c>
       <c r="F15">
-        <v>325496</v>
+        <v>190854</v>
       </c>
       <c r="G15">
         <f t="shared" si="0"/>
-        <v>47.435560350336999</v>
+        <v>49.878582279593282</v>
       </c>
       <c r="H15">
         <f t="shared" si="1"/>
-        <v>52.564439649663001</v>
+        <v>50.121417720406718</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
@@ -1013,21 +1019,21 @@
         <v>9981477</v>
       </c>
       <c r="D16">
-        <v>4973468</v>
+        <v>5223655</v>
       </c>
       <c r="E16">
-        <v>4973468</v>
+        <v>5223655</v>
       </c>
       <c r="F16">
-        <v>541262</v>
+        <v>303366</v>
       </c>
       <c r="G16">
         <f t="shared" si="0"/>
-        <v>49.82697450487538</v>
+        <v>52.333487318560167</v>
       </c>
       <c r="H16">
         <f t="shared" si="1"/>
-        <v>50.17302549512462</v>
+        <v>47.666512681439833</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
@@ -1041,21 +1047,21 @@
         <v>10117772</v>
       </c>
       <c r="D17">
-        <v>4639283</v>
+        <v>4899108</v>
       </c>
       <c r="E17">
-        <v>4639283</v>
+        <v>4899108</v>
       </c>
       <c r="F17">
-        <v>384144</v>
+        <v>224710</v>
       </c>
       <c r="G17">
         <f t="shared" si="0"/>
-        <v>45.852812259457913</v>
+        <v>48.420818338266564</v>
       </c>
       <c r="H17">
         <f t="shared" si="1"/>
-        <v>54.147187740542087</v>
+        <v>51.579181661733436</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
@@ -1069,21 +1075,21 @@
         <v>9190057</v>
       </c>
       <c r="D18">
-        <v>4485113</v>
+        <v>4735025</v>
       </c>
       <c r="E18">
-        <v>4485113</v>
+        <v>4735025</v>
       </c>
       <c r="F18">
-        <v>506812</v>
+        <v>318511</v>
       </c>
       <c r="G18">
         <f t="shared" si="0"/>
-        <v>48.803973685908588</v>
+        <v>51.523347461283429</v>
       </c>
       <c r="H18">
         <f t="shared" si="1"/>
-        <v>51.196026314091412</v>
+        <v>48.476652538716571</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
@@ -1097,21 +1103,21 @@
         <v>9215258</v>
       </c>
       <c r="D19">
-        <v>4096616</v>
+        <v>4324041</v>
       </c>
       <c r="E19">
-        <v>4096616</v>
+        <v>4324041</v>
       </c>
       <c r="F19">
-        <v>360844</v>
+        <v>216204</v>
       </c>
       <c r="G19">
         <f t="shared" si="0"/>
-        <v>44.454707616433531</v>
+        <v>46.922625497842816</v>
       </c>
       <c r="H19">
         <f t="shared" si="1"/>
-        <v>55.545292383566469</v>
+        <v>53.077374502157184</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
@@ -1125,21 +1131,21 @@
         <v>8855104</v>
       </c>
       <c r="D20">
-        <v>3905919</v>
+        <v>4143109</v>
       </c>
       <c r="E20">
-        <v>3905919</v>
+        <v>4143109</v>
       </c>
       <c r="F20">
-        <v>338622</v>
+        <v>208154</v>
       </c>
       <c r="G20">
         <f t="shared" si="0"/>
-        <v>44.109239146146678</v>
+        <v>46.787807348168919</v>
       </c>
       <c r="H20">
         <f t="shared" si="1"/>
-        <v>55.890760853853322</v>
+        <v>53.212192651831081</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
@@ -1153,21 +1159,21 @@
         <v>8480824</v>
       </c>
       <c r="D21">
-        <v>3821680</v>
+        <v>4032082</v>
       </c>
       <c r="E21">
-        <v>3821680</v>
+        <v>4032082</v>
       </c>
       <c r="F21">
-        <v>277592</v>
+        <v>164706</v>
       </c>
       <c r="G21">
         <f t="shared" si="0"/>
-        <v>45.062602407501913</v>
+        <v>47.543516997876623</v>
       </c>
       <c r="H21">
         <f t="shared" si="1"/>
-        <v>54.937397592498087</v>
+        <v>52.456483002123377</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
@@ -1181,21 +1187,21 @@
         <v>7881173</v>
       </c>
       <c r="D22">
-        <v>3512955</v>
+        <v>3708404</v>
       </c>
       <c r="E22">
-        <v>3512955</v>
+        <v>3708404</v>
       </c>
       <c r="F22">
-        <v>283216</v>
+        <v>171192</v>
       </c>
       <c r="G22">
         <f t="shared" si="0"/>
-        <v>44.574012015724058</v>
+        <v>47.05396011482047</v>
       </c>
       <c r="H22">
         <f t="shared" si="1"/>
-        <v>55.425987984275942</v>
+        <v>52.94603988517953</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
@@ -1209,21 +1215,21 @@
         <v>10540135</v>
       </c>
       <c r="D23">
-        <v>4998335</v>
+        <v>5266841</v>
       </c>
       <c r="E23">
-        <v>4998335</v>
+        <v>5266841</v>
       </c>
       <c r="F23">
-        <v>394256</v>
+        <v>239062</v>
       </c>
       <c r="G23">
         <f t="shared" si="0"/>
-        <v>47.421925810248162</v>
+        <v>49.969388437624374</v>
       </c>
       <c r="H23">
         <f t="shared" si="1"/>
-        <v>52.578074189751838</v>
+        <v>50.030611562375626</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
@@ -1237,21 +1243,21 @@
         <v>9377750</v>
       </c>
       <c r="D24">
-        <v>3995087</v>
+        <v>4247503</v>
       </c>
       <c r="E24">
-        <v>3995087</v>
+        <v>4247503</v>
       </c>
       <c r="F24">
-        <v>616184</v>
+        <v>399570</v>
       </c>
       <c r="G24">
         <f t="shared" si="0"/>
-        <v>42.601764815654072</v>
+        <v>45.293412598970967</v>
       </c>
       <c r="H24">
         <f t="shared" si="1"/>
-        <v>57.398235184345928</v>
+        <v>54.706587401029033</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
@@ -1265,21 +1271,21 @@
         <v>10013563</v>
       </c>
       <c r="D25">
-        <v>4715574</v>
+        <v>4981194</v>
       </c>
       <c r="E25">
-        <v>4715574</v>
+        <v>4981194</v>
       </c>
       <c r="F25">
-        <v>421738</v>
+        <v>243388</v>
       </c>
       <c r="G25">
         <f t="shared" si="0"/>
-        <v>47.091869297671565</v>
+        <v>49.74447157320526</v>
       </c>
       <c r="H25">
         <f t="shared" si="1"/>
-        <v>52.908130702328435</v>
+        <v>50.25552842679474</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
@@ -1293,21 +1299,21 @@
         <v>9130792</v>
       </c>
       <c r="D26">
-        <v>4104803</v>
+        <v>4327582</v>
       </c>
       <c r="E26">
-        <v>4104803</v>
+        <v>4327582</v>
       </c>
       <c r="F26">
-        <v>260364</v>
+        <v>165548</v>
       </c>
       <c r="G26">
         <f t="shared" si="0"/>
-        <v>44.955607355856969</v>
+        <v>47.395472375233169</v>
       </c>
       <c r="H26">
         <f t="shared" si="1"/>
-        <v>55.044392644143031</v>
+        <v>52.604527624766831</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
@@ -1321,21 +1327,21 @@
         <v>9429881</v>
       </c>
       <c r="D27">
-        <v>4258690</v>
+        <v>4484688</v>
       </c>
       <c r="E27">
-        <v>4258690</v>
+        <v>4484688</v>
       </c>
       <c r="F27">
-        <v>285240</v>
+        <v>178576</v>
       </c>
       <c r="G27">
         <f t="shared" si="0"/>
-        <v>45.161651562729162</v>
+        <v>47.558267172194434</v>
       </c>
       <c r="H27">
         <f t="shared" si="1"/>
-        <v>54.838348437270838</v>
+        <v>52.441732827805566</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
@@ -1349,21 +1355,21 @@
         <v>9525337</v>
       </c>
       <c r="D28">
-        <v>4376692</v>
+        <v>4628790</v>
       </c>
       <c r="E28">
-        <v>4376692</v>
+        <v>4628790</v>
       </c>
       <c r="F28">
-        <v>360568</v>
+        <v>213598</v>
       </c>
       <c r="G28">
         <f t="shared" si="0"/>
-        <v>45.947896646596334</v>
+        <v>48.594501170929703</v>
       </c>
       <c r="H28">
         <f t="shared" si="1"/>
-        <v>54.052103353403666</v>
+        <v>51.405498829070297</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.35">
@@ -1377,21 +1383,21 @@
         <v>10261218</v>
       </c>
       <c r="D29">
-        <v>4579738</v>
+        <v>4822141</v>
       </c>
       <c r="E29">
-        <v>4579738</v>
+        <v>4822141</v>
       </c>
       <c r="F29">
-        <v>270182</v>
+        <v>168756</v>
       </c>
       <c r="G29">
         <f t="shared" si="0"/>
-        <v>44.631524249850258</v>
+        <v>46.993846149648121</v>
       </c>
       <c r="H29">
         <f t="shared" si="1"/>
-        <v>55.368475750149742</v>
+        <v>53.006153850351879</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
@@ -1405,21 +1411,21 @@
         <v>8753321</v>
       </c>
       <c r="D30">
-        <v>4017325</v>
+        <v>4254092</v>
       </c>
       <c r="E30">
-        <v>4017325</v>
+        <v>4254092</v>
       </c>
       <c r="F30">
-        <v>352810</v>
+        <v>214444</v>
       </c>
       <c r="G30">
         <f t="shared" si="0"/>
-        <v>45.894866645470898</v>
+        <v>48.599748598274871</v>
       </c>
       <c r="H30">
         <f t="shared" si="1"/>
-        <v>54.105133354529102</v>
+        <v>51.400251401725129</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
@@ -1433,21 +1439,21 @@
         <v>8658165</v>
       </c>
       <c r="D31">
-        <v>4115501</v>
+        <v>4339777</v>
       </c>
       <c r="E31">
-        <v>4115501</v>
+        <v>4339777</v>
       </c>
       <c r="F31">
-        <v>281134</v>
+        <v>169296</v>
       </c>
       <c r="G31">
         <f t="shared" si="0"/>
-        <v>47.533178219634301</v>
+        <v>50.12351924455124</v>
       </c>
       <c r="H31">
         <f t="shared" si="1"/>
-        <v>52.466821780365699</v>
+        <v>49.87648075544876</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.35">
@@ -1461,21 +1467,21 @@
         <v>9588630</v>
       </c>
       <c r="D32">
-        <v>4909746</v>
+        <v>5179268</v>
       </c>
       <c r="E32">
-        <v>4909746</v>
+        <v>5179268</v>
       </c>
       <c r="F32">
-        <v>741399</v>
+        <v>468916</v>
       </c>
       <c r="G32">
         <f t="shared" si="0"/>
-        <v>51.203832038570681</v>
+        <v>54.014681972294269</v>
       </c>
       <c r="H32">
         <f t="shared" si="1"/>
-        <v>48.796167961429319</v>
+        <v>45.985318027705731</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.35">
@@ -1489,21 +1495,21 @@
         <v>11481612</v>
       </c>
       <c r="D33">
-        <v>5379881</v>
+        <v>5663014</v>
       </c>
       <c r="E33">
-        <v>5379881</v>
+        <v>5663014</v>
       </c>
       <c r="F33">
-        <v>571490</v>
+        <v>314102</v>
       </c>
       <c r="G33">
         <f t="shared" si="0"/>
-        <v>46.856495411968282</v>
+        <v>49.322464476242537</v>
       </c>
       <c r="H33">
         <f t="shared" si="1"/>
-        <v>53.143504588031718</v>
+        <v>50.677535523757463</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.35">
@@ -1517,21 +1523,21 @@
         <v>10199511</v>
       </c>
       <c r="D34">
-        <v>4866725</v>
+        <v>5126136</v>
       </c>
       <c r="E34">
-        <v>4866725</v>
+        <v>5126136</v>
       </c>
       <c r="F34">
-        <v>644392</v>
+        <v>352150</v>
       </c>
       <c r="G34">
         <f t="shared" si="0"/>
-        <v>47.715277722628073</v>
+        <v>50.258644752674911</v>
       </c>
       <c r="H34">
         <f t="shared" si="1"/>
-        <v>52.284722277371927</v>
+        <v>49.741355247325089</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.35">
@@ -1545,21 +1551,21 @@
         <v>8902663</v>
       </c>
       <c r="D35">
-        <v>4490908</v>
+        <v>4717970</v>
       </c>
       <c r="E35">
-        <v>4490908</v>
+        <v>4717970</v>
       </c>
       <c r="F35">
-        <v>328884</v>
+        <v>190812</v>
       </c>
       <c r="G35">
         <f t="shared" si="0"/>
-        <v>50.444546760896152</v>
+        <v>52.995042045284656</v>
       </c>
       <c r="H35">
         <f t="shared" si="1"/>
-        <v>49.555453239103848</v>
+        <v>47.004957954715344</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.35">
@@ -1573,21 +1579,21 @@
         <v>11534227</v>
       </c>
       <c r="D36">
-        <v>5255157</v>
+        <v>5552366</v>
       </c>
       <c r="E36">
-        <v>5255157</v>
+        <v>5552366</v>
       </c>
       <c r="F36">
-        <v>735976</v>
+        <v>412022</v>
       </c>
       <c r="G36">
         <f t="shared" si="0"/>
-        <v>45.561414735465149</v>
+        <v>48.138171721433956</v>
       </c>
       <c r="H36">
         <f t="shared" si="1"/>
-        <v>54.438585264534851</v>
+        <v>51.861828278566044</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.35">
@@ -1601,21 +1607,21 @@
         <v>10601036</v>
       </c>
       <c r="D37">
-        <v>5322470</v>
+        <v>5583984</v>
       </c>
       <c r="E37">
-        <v>5322470</v>
+        <v>5583984</v>
       </c>
       <c r="F37">
-        <v>500072</v>
+        <v>269242</v>
       </c>
       <c r="G37">
         <f t="shared" si="0"/>
-        <v>50.207074101059554</v>
+        <v>52.673946206766963</v>
       </c>
       <c r="H37">
         <f t="shared" si="1"/>
-        <v>49.792925898940446</v>
+        <v>47.326053793233037</v>
       </c>
     </row>
   </sheetData>
@@ -1627,824 +1633,827 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="7" max="7" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="5" width="8.7265625" style="1"/>
+    <col min="6" max="6" width="22.26953125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>44104080</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>44104080</v>
       </c>
-      <c r="D2">
-        <v>25981615</v>
-      </c>
-      <c r="E2">
-        <v>25981615</v>
-      </c>
-      <c r="F2">
-        <v>30839660</v>
-      </c>
-      <c r="G2">
+      <c r="D2" s="1">
+        <v>29726641</v>
+      </c>
+      <c r="E2" s="1">
+        <v>29726641</v>
+      </c>
+      <c r="F2" s="1">
+        <v>23722182</v>
+      </c>
+      <c r="G2" s="1">
         <f>(D2*100)/B2</f>
-        <v>58.90977660116706</v>
-      </c>
-      <c r="H2">
+        <v>67.401113457076988</v>
+      </c>
+      <c r="H2" s="1">
         <f>100-G2</f>
-        <v>41.09022339883294</v>
+        <v>32.598886542923012</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>26843136</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>26843136</v>
       </c>
-      <c r="D3">
-        <v>15156824</v>
-      </c>
-      <c r="E3">
-        <v>15156824</v>
-      </c>
-      <c r="F3">
-        <v>21022578</v>
-      </c>
-      <c r="G3">
+      <c r="D3" s="1">
+        <v>17723103</v>
+      </c>
+      <c r="E3" s="1">
+        <v>17723103</v>
+      </c>
+      <c r="F3" s="1">
+        <v>16447805</v>
+      </c>
+      <c r="G3" s="1">
         <f t="shared" ref="G3:G29" si="0">(D3*100)/B3</f>
-        <v>56.46443098153658</v>
-      </c>
-      <c r="H3">
+        <v>66.024711121681165</v>
+      </c>
+      <c r="H3" s="1">
         <f t="shared" ref="H3:H29" si="1">100-G3</f>
-        <v>43.53556901846342</v>
+        <v>33.975288878318835</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>39767058</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>39767058</v>
       </c>
-      <c r="D4">
-        <v>23797092</v>
-      </c>
-      <c r="E4">
-        <v>23797092</v>
-      </c>
-      <c r="F4">
-        <v>26339480</v>
-      </c>
-      <c r="G4">
-        <f t="shared" si="0"/>
-        <v>59.841218326988134</v>
-      </c>
-      <c r="H4">
-        <f t="shared" si="1"/>
-        <v>40.158781673011866</v>
+      <c r="D4" s="1">
+        <v>27131664</v>
+      </c>
+      <c r="E4" s="1">
+        <v>27131664</v>
+      </c>
+      <c r="F4" s="1">
+        <v>19881792</v>
+      </c>
+      <c r="G4" s="1">
+        <f t="shared" si="0"/>
+        <v>68.226480319464414</v>
+      </c>
+      <c r="H4" s="1">
+        <f t="shared" si="1"/>
+        <v>31.773519680535586</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>28964924</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>28964924</v>
       </c>
-      <c r="D5">
-        <v>15382904</v>
-      </c>
-      <c r="E5">
-        <v>15382904</v>
-      </c>
-      <c r="F5">
-        <v>19212438</v>
-      </c>
-      <c r="G5">
-        <f t="shared" si="0"/>
-        <v>53.108732479325681</v>
-      </c>
-      <c r="H5">
-        <f t="shared" si="1"/>
-        <v>46.891267520674319</v>
+      <c r="D5" s="1">
+        <v>17809190</v>
+      </c>
+      <c r="E5" s="1">
+        <v>17809190</v>
+      </c>
+      <c r="F5" s="1">
+        <v>14913217</v>
+      </c>
+      <c r="G5" s="1">
+        <f t="shared" si="0"/>
+        <v>61.485367612219527</v>
+      </c>
+      <c r="H5" s="1">
+        <f t="shared" si="1"/>
+        <v>38.514632387780473</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>30177602</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <v>30177602</v>
       </c>
-      <c r="D6">
-        <v>16695055</v>
-      </c>
-      <c r="E6">
-        <v>16695055</v>
-      </c>
-      <c r="F6">
-        <v>24432006</v>
-      </c>
-      <c r="G6">
-        <f t="shared" si="0"/>
-        <v>55.322669442058384</v>
-      </c>
-      <c r="H6">
-        <f t="shared" si="1"/>
-        <v>44.677330557941616</v>
+      <c r="D6" s="1">
+        <v>19571517</v>
+      </c>
+      <c r="E6" s="1">
+        <v>19571517</v>
+      </c>
+      <c r="F6" s="1">
+        <v>19460165</v>
+      </c>
+      <c r="G6" s="1">
+        <f t="shared" si="0"/>
+        <v>64.854447348069598</v>
+      </c>
+      <c r="H6" s="1">
+        <f t="shared" si="1"/>
+        <v>35.145552651930402</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <v>24646853</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="1">
         <v>24646853</v>
       </c>
-      <c r="D7">
-        <v>14133299</v>
-      </c>
-      <c r="E7">
-        <v>14133299</v>
-      </c>
-      <c r="F7">
-        <v>18326300</v>
-      </c>
-      <c r="G7">
-        <f t="shared" si="0"/>
-        <v>57.343219436574721</v>
-      </c>
-      <c r="H7">
-        <f t="shared" si="1"/>
-        <v>42.656780563425279</v>
+      <c r="D7" s="1">
+        <v>16271977</v>
+      </c>
+      <c r="E7" s="1">
+        <v>16271977</v>
+      </c>
+      <c r="F7" s="1">
+        <v>14646575</v>
+      </c>
+      <c r="G7" s="1">
+        <f t="shared" si="0"/>
+        <v>66.020505741645806</v>
+      </c>
+      <c r="H7" s="1">
+        <f t="shared" si="1"/>
+        <v>33.979494258354194</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
         <v>31415272</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="1">
         <v>31415272</v>
       </c>
-      <c r="D8">
-        <v>16966223</v>
-      </c>
-      <c r="E8">
-        <v>16966223</v>
-      </c>
-      <c r="F8">
-        <v>23899764</v>
-      </c>
-      <c r="G8">
-        <f t="shared" si="0"/>
-        <v>54.00629031637861</v>
-      </c>
-      <c r="H8">
-        <f t="shared" si="1"/>
-        <v>45.99370968362139</v>
+      <c r="D8" s="1">
+        <v>19850185</v>
+      </c>
+      <c r="E8" s="1">
+        <v>19850185</v>
+      </c>
+      <c r="F8" s="1">
+        <v>18892536</v>
+      </c>
+      <c r="G8" s="1">
+        <f t="shared" si="0"/>
+        <v>63.186417739754091</v>
+      </c>
+      <c r="H8" s="1">
+        <f t="shared" si="1"/>
+        <v>36.813582260245909</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1">
         <v>30206664</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="1">
         <v>30206664</v>
       </c>
-      <c r="D9">
-        <v>15769761</v>
-      </c>
-      <c r="E9">
-        <v>15769761</v>
-      </c>
-      <c r="F9">
-        <v>26086551</v>
-      </c>
-      <c r="G9">
-        <f t="shared" si="0"/>
-        <v>52.206231710989336</v>
-      </c>
-      <c r="H9">
-        <f t="shared" si="1"/>
-        <v>47.793768289010664</v>
+      <c r="D9" s="1">
+        <v>18796231</v>
+      </c>
+      <c r="E9" s="1">
+        <v>18796231</v>
+      </c>
+      <c r="F9" s="1">
+        <v>20756366</v>
+      </c>
+      <c r="G9" s="1">
+        <f t="shared" si="0"/>
+        <v>62.225444689953186</v>
+      </c>
+      <c r="H9" s="1">
+        <f t="shared" si="1"/>
+        <v>37.774555310046814</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="1">
         <v>31819911</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="1">
         <v>31819911</v>
       </c>
-      <c r="D10">
-        <v>18289228</v>
-      </c>
-      <c r="E10">
-        <v>18289228</v>
-      </c>
-      <c r="F10">
-        <v>22421046</v>
-      </c>
-      <c r="G10">
-        <f t="shared" si="0"/>
-        <v>57.47730721182721</v>
-      </c>
-      <c r="H10">
-        <f t="shared" si="1"/>
-        <v>42.52269278817279</v>
+      <c r="D10" s="1">
+        <v>20955285</v>
+      </c>
+      <c r="E10" s="1">
+        <v>20955285</v>
+      </c>
+      <c r="F10" s="1">
+        <v>17474776</v>
+      </c>
+      <c r="G10" s="1">
+        <f t="shared" si="0"/>
+        <v>65.855888157575293</v>
+      </c>
+      <c r="H10" s="1">
+        <f t="shared" si="1"/>
+        <v>34.144111842424707</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1">
         <v>24445510</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="1">
         <v>24445510</v>
       </c>
-      <c r="D11">
-        <v>12681424</v>
-      </c>
-      <c r="E11">
-        <v>12681424</v>
-      </c>
-      <c r="F11">
-        <v>16800710</v>
-      </c>
-      <c r="G11">
-        <f t="shared" si="0"/>
-        <v>51.876291392570657</v>
-      </c>
-      <c r="H11">
-        <f t="shared" si="1"/>
-        <v>48.123708607429343</v>
+      <c r="D11" s="1">
+        <v>14539383</v>
+      </c>
+      <c r="E11" s="1">
+        <v>14539383</v>
+      </c>
+      <c r="F11" s="1">
+        <v>13548474</v>
+      </c>
+      <c r="G11" s="1">
+        <f t="shared" si="0"/>
+        <v>59.476701447423267</v>
+      </c>
+      <c r="H11" s="1">
+        <f t="shared" si="1"/>
+        <v>40.523298552576733</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+      <c r="A12" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="1">
         <v>29927066</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="1">
         <v>29927066</v>
       </c>
-      <c r="D12">
-        <v>19134216</v>
-      </c>
-      <c r="E12">
-        <v>19134216</v>
-      </c>
-      <c r="F12">
-        <v>18858769</v>
-      </c>
-      <c r="G12">
-        <f t="shared" si="0"/>
-        <v>63.936157323273854</v>
-      </c>
-      <c r="H12">
-        <f t="shared" si="1"/>
-        <v>36.063842676726146</v>
+      <c r="D12" s="1">
+        <v>21570067</v>
+      </c>
+      <c r="E12" s="1">
+        <v>21570067</v>
+      </c>
+      <c r="F12" s="1">
+        <v>13757630</v>
+      </c>
+      <c r="G12" s="1">
+        <f t="shared" si="0"/>
+        <v>72.075448358352276</v>
+      </c>
+      <c r="H12" s="1">
+        <f t="shared" si="1"/>
+        <v>27.924551641647724</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+      <c r="A13" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="1">
         <v>32381027</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="1">
         <v>32381027</v>
       </c>
-      <c r="D13">
-        <v>18665949</v>
-      </c>
-      <c r="E13">
-        <v>18665949</v>
-      </c>
-      <c r="F13">
-        <v>23829077</v>
-      </c>
-      <c r="G13">
-        <f t="shared" si="0"/>
-        <v>57.644709662852883</v>
-      </c>
-      <c r="H13">
-        <f t="shared" si="1"/>
-        <v>42.355290337147117</v>
+      <c r="D13" s="1">
+        <v>21518913</v>
+      </c>
+      <c r="E13" s="1">
+        <v>21518913</v>
+      </c>
+      <c r="F13" s="1">
+        <v>18800698</v>
+      </c>
+      <c r="G13" s="1">
+        <f t="shared" si="0"/>
+        <v>66.45531347724085</v>
+      </c>
+      <c r="H13" s="1">
+        <f t="shared" si="1"/>
+        <v>33.54468652275915</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+      <c r="A14" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="1">
         <v>29059690</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="1">
         <v>29059690</v>
       </c>
-      <c r="D14">
-        <v>16295779</v>
-      </c>
-      <c r="E14">
-        <v>16295779</v>
-      </c>
-      <c r="F14">
-        <v>17457386</v>
-      </c>
-      <c r="G14">
-        <f t="shared" si="0"/>
-        <v>56.076919609259427</v>
-      </c>
-      <c r="H14">
-        <f t="shared" si="1"/>
-        <v>43.923080390740573</v>
+      <c r="D14" s="1">
+        <v>18546542</v>
+      </c>
+      <c r="E14" s="1">
+        <v>18546542</v>
+      </c>
+      <c r="F14" s="1">
+        <v>13471909</v>
+      </c>
+      <c r="G14" s="1">
+        <f t="shared" si="0"/>
+        <v>63.822229349315151</v>
+      </c>
+      <c r="H14" s="1">
+        <f t="shared" si="1"/>
+        <v>36.177770650684849</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+      <c r="A15" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="1">
         <v>30032397</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="1">
         <v>30032397</v>
       </c>
-      <c r="D15">
-        <v>17381258</v>
-      </c>
-      <c r="E15">
-        <v>17381258</v>
-      </c>
-      <c r="F15">
-        <v>25183491</v>
-      </c>
-      <c r="G15">
-        <f t="shared" si="0"/>
-        <v>57.875027424550893</v>
-      </c>
-      <c r="H15">
-        <f t="shared" si="1"/>
-        <v>42.124972575449107</v>
+      <c r="D15" s="1">
+        <v>20349981</v>
+      </c>
+      <c r="E15" s="1">
+        <v>20349981</v>
+      </c>
+      <c r="F15" s="1">
+        <v>19883653</v>
+      </c>
+      <c r="G15" s="1">
+        <f t="shared" si="0"/>
+        <v>67.760095872467318</v>
+      </c>
+      <c r="H15" s="1">
+        <f t="shared" si="1"/>
+        <v>32.239904127532682</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+      <c r="A16" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="1">
         <v>27648758</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="1">
         <v>27648758</v>
       </c>
-      <c r="D16">
-        <v>15669825</v>
-      </c>
-      <c r="E16">
-        <v>15669825</v>
-      </c>
-      <c r="F16">
-        <v>20667496</v>
-      </c>
-      <c r="G16">
-        <f t="shared" si="0"/>
-        <v>56.674607228288515</v>
-      </c>
-      <c r="H16">
-        <f t="shared" si="1"/>
-        <v>43.325392771711485</v>
+      <c r="D16" s="1">
+        <v>18130011</v>
+      </c>
+      <c r="E16" s="1">
+        <v>18130011</v>
+      </c>
+      <c r="F16" s="1">
+        <v>16298481</v>
+      </c>
+      <c r="G16" s="1">
+        <f t="shared" si="0"/>
+        <v>65.572605467486099</v>
+      </c>
+      <c r="H16" s="1">
+        <f t="shared" si="1"/>
+        <v>34.427394532513901</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+      <c r="A17" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="1">
         <v>27834839</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="1">
         <v>27834839</v>
       </c>
-      <c r="D17">
-        <v>13615911</v>
-      </c>
-      <c r="E17">
-        <v>13615911</v>
-      </c>
-      <c r="F17">
-        <v>21157553</v>
-      </c>
-      <c r="G17">
-        <f t="shared" si="0"/>
-        <v>48.916794525019526</v>
-      </c>
-      <c r="H17">
-        <f t="shared" si="1"/>
-        <v>51.083205474980474</v>
+      <c r="D17" s="1">
+        <v>15918629</v>
+      </c>
+      <c r="E17" s="1">
+        <v>15918629</v>
+      </c>
+      <c r="F17" s="1">
+        <v>19190286</v>
+      </c>
+      <c r="G17" s="1">
+        <f t="shared" si="0"/>
+        <v>57.189585325066908</v>
+      </c>
+      <c r="H17" s="1">
+        <f t="shared" si="1"/>
+        <v>42.810414674933092</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+      <c r="A18" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="1">
         <v>33106734</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="1">
         <v>33106734</v>
       </c>
-      <c r="D18">
-        <v>18309522</v>
-      </c>
-      <c r="E18">
-        <v>18309522</v>
-      </c>
-      <c r="F18">
-        <v>25557957</v>
-      </c>
-      <c r="G18">
-        <f t="shared" si="0"/>
-        <v>55.30452505523499</v>
-      </c>
-      <c r="H18">
-        <f t="shared" si="1"/>
-        <v>44.69547494476501</v>
+      <c r="D18" s="1">
+        <v>21349241</v>
+      </c>
+      <c r="E18" s="1">
+        <v>21349241</v>
+      </c>
+      <c r="F18" s="1">
+        <v>20310070</v>
+      </c>
+      <c r="G18" s="1">
+        <f t="shared" si="0"/>
+        <v>64.486098205881618</v>
+      </c>
+      <c r="H18" s="1">
+        <f t="shared" si="1"/>
+        <v>35.513901794118382</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
+      <c r="A19" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="1">
         <v>26791740</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="1">
         <v>26791740</v>
       </c>
-      <c r="D19">
-        <v>14226162</v>
-      </c>
-      <c r="E19">
-        <v>14226162</v>
-      </c>
-      <c r="F19">
-        <v>20520859</v>
-      </c>
-      <c r="G19">
-        <f t="shared" si="0"/>
-        <v>53.099059635544386</v>
-      </c>
-      <c r="H19">
-        <f t="shared" si="1"/>
-        <v>46.900940364455614</v>
+      <c r="D19" s="1">
+        <v>16512773</v>
+      </c>
+      <c r="E19" s="1">
+        <v>16512773</v>
+      </c>
+      <c r="F19" s="1">
+        <v>16658758</v>
+      </c>
+      <c r="G19" s="1">
+        <f t="shared" si="0"/>
+        <v>61.633820722356965</v>
+      </c>
+      <c r="H19" s="1">
+        <f t="shared" si="1"/>
+        <v>38.366179277643035</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
+      <c r="A20" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="1">
         <v>31302866</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="1">
         <v>31302866</v>
       </c>
-      <c r="D20">
-        <v>17733714</v>
-      </c>
-      <c r="E20">
-        <v>17733714</v>
-      </c>
-      <c r="F20">
-        <v>23401601</v>
-      </c>
-      <c r="G20">
-        <f t="shared" si="0"/>
-        <v>56.652045854203891</v>
-      </c>
-      <c r="H20">
-        <f t="shared" si="1"/>
-        <v>43.347954145796109</v>
+      <c r="D20" s="1">
+        <v>20702257</v>
+      </c>
+      <c r="E20" s="1">
+        <v>20702257</v>
+      </c>
+      <c r="F20" s="1">
+        <v>18322344</v>
+      </c>
+      <c r="G20" s="1">
+        <f t="shared" si="0"/>
+        <v>66.135340450935061</v>
+      </c>
+      <c r="H20" s="1">
+        <f t="shared" si="1"/>
+        <v>33.864659549064939</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
+      <c r="A21" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="1">
         <v>27023641</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="1">
         <v>27023641</v>
       </c>
-      <c r="D21">
-        <v>15006094</v>
-      </c>
-      <c r="E21">
-        <v>15006094</v>
-      </c>
-      <c r="F21">
-        <v>19923352</v>
-      </c>
-      <c r="G21">
-        <f t="shared" si="0"/>
-        <v>55.5295047029377</v>
-      </c>
-      <c r="H21">
-        <f t="shared" si="1"/>
-        <v>44.4704952970623</v>
+      <c r="D21" s="1">
+        <v>17344757</v>
+      </c>
+      <c r="E21" s="1">
+        <v>17344757</v>
+      </c>
+      <c r="F21" s="1">
+        <v>15726159</v>
+      </c>
+      <c r="G21" s="1">
+        <f t="shared" si="0"/>
+        <v>64.1836420192231</v>
+      </c>
+      <c r="H21" s="1">
+        <f t="shared" si="1"/>
+        <v>35.8163579807769</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
+      <c r="A22" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="1">
         <v>28294978</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="1">
         <v>28294978</v>
       </c>
-      <c r="D22">
-        <v>16022703</v>
-      </c>
-      <c r="E22">
-        <v>16022703</v>
-      </c>
-      <c r="F22">
-        <v>23247836</v>
-      </c>
-      <c r="G22">
-        <f t="shared" si="0"/>
-        <v>56.627373946005541</v>
-      </c>
-      <c r="H22">
-        <f t="shared" si="1"/>
-        <v>43.372626053994459</v>
+      <c r="D22" s="1">
+        <v>18782523</v>
+      </c>
+      <c r="E22" s="1">
+        <v>18782523</v>
+      </c>
+      <c r="F22" s="1">
+        <v>18480713</v>
+      </c>
+      <c r="G22" s="1">
+        <f t="shared" si="0"/>
+        <v>66.381118939198331</v>
+      </c>
+      <c r="H22" s="1">
+        <f t="shared" si="1"/>
+        <v>33.618881060801669</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
+      <c r="A23" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="1">
         <v>33593329</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="1">
         <v>33593329</v>
       </c>
-      <c r="D23">
-        <v>19333677</v>
-      </c>
-      <c r="E23">
-        <v>19333677</v>
-      </c>
-      <c r="F23">
-        <v>25419154</v>
-      </c>
-      <c r="G23">
-        <f t="shared" si="0"/>
-        <v>57.552131853321235</v>
-      </c>
-      <c r="H23">
-        <f t="shared" si="1"/>
-        <v>42.447868146678765</v>
+      <c r="D23" s="1">
+        <v>22397536</v>
+      </c>
+      <c r="E23" s="1">
+        <v>22397536</v>
+      </c>
+      <c r="F23" s="1">
+        <v>19904894</v>
+      </c>
+      <c r="G23" s="1">
+        <f t="shared" si="0"/>
+        <v>66.672570616624512</v>
+      </c>
+      <c r="H23" s="1">
+        <f t="shared" si="1"/>
+        <v>33.327429383375488</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
+      <c r="A24" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="1">
         <v>31105749</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="1">
         <v>31105749</v>
       </c>
-      <c r="D24">
-        <v>16664812</v>
-      </c>
-      <c r="E24">
-        <v>16664812</v>
-      </c>
-      <c r="F24">
-        <v>22790827</v>
-      </c>
-      <c r="G24">
-        <f t="shared" si="0"/>
-        <v>53.574700933901319</v>
-      </c>
-      <c r="H24">
-        <f t="shared" si="1"/>
-        <v>46.425299066098681</v>
+      <c r="D24" s="1">
+        <v>19454576</v>
+      </c>
+      <c r="E24" s="1">
+        <v>19454576</v>
+      </c>
+      <c r="F24" s="1">
+        <v>17949690</v>
+      </c>
+      <c r="G24" s="1">
+        <f t="shared" si="0"/>
+        <v>62.543345283214364</v>
+      </c>
+      <c r="H24" s="1">
+        <f t="shared" si="1"/>
+        <v>37.456654716785636</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
+      <c r="A25" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="1">
         <v>25239430</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="1">
         <v>25239430</v>
       </c>
-      <c r="D25">
-        <v>14239767</v>
-      </c>
-      <c r="E25">
-        <v>14239767</v>
-      </c>
-      <c r="F25">
-        <v>20530517</v>
-      </c>
-      <c r="G25">
-        <f t="shared" si="0"/>
-        <v>56.418734495985049</v>
-      </c>
-      <c r="H25">
-        <f t="shared" si="1"/>
-        <v>43.581265504014951</v>
+      <c r="D25" s="1">
+        <v>16592578</v>
+      </c>
+      <c r="E25" s="1">
+        <v>16592578</v>
+      </c>
+      <c r="F25" s="1">
+        <v>16374948</v>
+      </c>
+      <c r="G25" s="1">
+        <f t="shared" si="0"/>
+        <v>65.740700166366679</v>
+      </c>
+      <c r="H25" s="1">
+        <f t="shared" si="1"/>
+        <v>34.259299833633321</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
+      <c r="A26" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="1">
         <v>33148390</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="1">
         <v>33148390</v>
       </c>
-      <c r="D26">
-        <v>18822785</v>
-      </c>
-      <c r="E26">
-        <v>18822785</v>
-      </c>
-      <c r="F26">
-        <v>25283264</v>
-      </c>
-      <c r="G26">
-        <f t="shared" si="0"/>
-        <v>56.783406373582551</v>
-      </c>
-      <c r="H26">
-        <f t="shared" si="1"/>
-        <v>43.216593626417449</v>
+      <c r="D26" s="1">
+        <v>21843996</v>
+      </c>
+      <c r="E26" s="1">
+        <v>21843996</v>
+      </c>
+      <c r="F26" s="1">
+        <v>19993210</v>
+      </c>
+      <c r="G26" s="1">
+        <f t="shared" si="0"/>
+        <v>65.897607696784064</v>
+      </c>
+      <c r="H26" s="1">
+        <f t="shared" si="1"/>
+        <v>34.102392303215936</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
+      <c r="A27" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="1">
         <v>29634371</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="1">
         <v>29634371</v>
       </c>
-      <c r="D27">
-        <v>16489958</v>
-      </c>
-      <c r="E27">
-        <v>16489958</v>
-      </c>
-      <c r="F27">
-        <v>22165882</v>
-      </c>
-      <c r="G27">
-        <f t="shared" si="0"/>
-        <v>55.644703914923653</v>
-      </c>
-      <c r="H27">
-        <f t="shared" si="1"/>
-        <v>44.355296085076347</v>
+      <c r="D27" s="1">
+        <v>19149279</v>
+      </c>
+      <c r="E27" s="1">
+        <v>19149279</v>
+      </c>
+      <c r="F27" s="1">
+        <v>17735880</v>
+      </c>
+      <c r="G27" s="1">
+        <f t="shared" si="0"/>
+        <v>64.618476295650069</v>
+      </c>
+      <c r="H27" s="1">
+        <f t="shared" si="1"/>
+        <v>35.381523704349931</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
+      <c r="A28" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="1">
         <v>37005211</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="1">
         <v>37005211</v>
       </c>
-      <c r="D28">
-        <v>21664945</v>
-      </c>
-      <c r="E28">
-        <v>21664945</v>
-      </c>
-      <c r="F28">
-        <v>30048919</v>
-      </c>
-      <c r="G28">
-        <f t="shared" si="0"/>
-        <v>58.545659961241675</v>
-      </c>
-      <c r="H28">
-        <f t="shared" si="1"/>
-        <v>41.454340038758325</v>
+      <c r="D28" s="1">
+        <v>25251769</v>
+      </c>
+      <c r="E28" s="1">
+        <v>25251769</v>
+      </c>
+      <c r="F28" s="1">
+        <v>23641873</v>
+      </c>
+      <c r="G28" s="1">
+        <f t="shared" si="0"/>
+        <v>68.238413773670956</v>
+      </c>
+      <c r="H28" s="1">
+        <f t="shared" si="1"/>
+        <v>31.761586226329044</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
+      <c r="A29" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="1">
         <v>25479196</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="1">
         <v>25479196</v>
       </c>
-      <c r="D29">
-        <v>14068144</v>
-      </c>
-      <c r="E29">
-        <v>14068144</v>
-      </c>
-      <c r="F29">
-        <v>19598330</v>
-      </c>
-      <c r="G29">
-        <f t="shared" si="0"/>
-        <v>55.214238314270197</v>
-      </c>
-      <c r="H29">
-        <f t="shared" si="1"/>
-        <v>44.785761685729803</v>
+      <c r="D29" s="1">
+        <v>16411783</v>
+      </c>
+      <c r="E29" s="1">
+        <v>16411783</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G29" s="1">
+        <f t="shared" si="0"/>
+        <v>64.412483816208336</v>
+      </c>
+      <c r="H29" s="1">
+        <f t="shared" si="1"/>
+        <v>35.587516183791664</v>
       </c>
     </row>
   </sheetData>

</xml_diff>